<commit_message>
Change text Josep to Moses
</commit_message>
<xml_diff>
--- a/data/allemand.xlsx
+++ b/data/allemand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -4262,8 +4262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4921,7 +4921,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>123</v>

</xml_diff>